<commit_message>
Rename CLOCK and RESET collumns
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -12,27 +12,20 @@
     <sheet name="Memo" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1" iterateDelta="0.0001"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <name val="Aptos Narrow"/>
       <charset val="129"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <charset val="129"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -133,22 +126,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -162,40 +161,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -605,19 +599,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="5.5" customWidth="1" style="20" min="1" max="1"/>
-    <col width="20.59765625" bestFit="1" customWidth="1" style="20" min="2" max="2"/>
-    <col width="15.5" bestFit="1" customWidth="1" style="20" min="3" max="3"/>
-    <col width="24.3984375" customWidth="1" style="20" min="4" max="4"/>
-    <col width="9.19921875" bestFit="1" customWidth="1" style="20" min="6" max="6"/>
-    <col width="36.8984375" bestFit="1" customWidth="1" style="20" min="7" max="7"/>
-    <col width="17.09765625" bestFit="1" customWidth="1" style="20" min="8" max="8"/>
-    <col width="74.09765625" customWidth="1" style="20" min="9" max="9"/>
-    <col width="64.69921875" bestFit="1" customWidth="1" style="20" min="10" max="10"/>
-    <col width="16.19921875" customWidth="1" style="20" min="11" max="11"/>
-    <col width="20.09765625" bestFit="1" customWidth="1" style="20" min="12" max="12"/>
-    <col width="18.3984375" bestFit="1" customWidth="1" style="20" min="13" max="13"/>
-    <col width="16.19921875" customWidth="1" style="20" min="14" max="15"/>
+    <col width="5.5" customWidth="1" style="21" min="1" max="1"/>
+    <col width="20.59765625" bestFit="1" customWidth="1" style="21" min="2" max="2"/>
+    <col width="15.5" bestFit="1" customWidth="1" style="21" min="3" max="3"/>
+    <col width="24.3984375" customWidth="1" style="21" min="4" max="4"/>
+    <col width="9.19921875" bestFit="1" customWidth="1" style="21" min="6" max="6"/>
+    <col width="36.8984375" bestFit="1" customWidth="1" style="21" min="7" max="7"/>
+    <col width="17.09765625" bestFit="1" customWidth="1" style="21" min="8" max="8"/>
+    <col width="74.09765625" customWidth="1" style="21" min="9" max="9"/>
+    <col width="64.69921875" bestFit="1" customWidth="1" style="21" min="10" max="10"/>
+    <col width="16.19921875" customWidth="1" style="21" min="11" max="11"/>
+    <col width="20.09765625" bestFit="1" customWidth="1" style="21" min="12" max="12"/>
+    <col width="18.3984375" bestFit="1" customWidth="1" style="21" min="13" max="13"/>
+    <col width="16.19921875" customWidth="1" style="21" min="14" max="15"/>
   </cols>
   <sheetData>
     <row r="2" ht="28.8" customFormat="1" customHeight="1" s="1">
@@ -795,316 +789,325 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A2:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="8.09765625" bestFit="1" customWidth="1" style="20" min="1" max="1"/>
-    <col width="12.09765625" bestFit="1" customWidth="1" style="20" min="2" max="2"/>
-    <col width="9.09765625" bestFit="1" customWidth="1" style="20" min="3" max="3"/>
-    <col width="9.796875" bestFit="1" customWidth="1" style="20" min="4" max="4"/>
-    <col width="18.296875" bestFit="1" customWidth="1" style="20" min="5" max="5"/>
-    <col width="16.19921875" bestFit="1" customWidth="1" style="20" min="6" max="6"/>
-    <col width="15.8984375" bestFit="1" customWidth="1" style="20" min="7" max="7"/>
-    <col width="21.69921875" bestFit="1" customWidth="1" style="20" min="8" max="8"/>
-    <col width="21.59765625" bestFit="1" customWidth="1" style="20" min="9" max="9"/>
-    <col width="11.8984375" bestFit="1" customWidth="1" style="20" min="10" max="10"/>
-    <col width="15.69921875" bestFit="1" customWidth="1" style="20" min="11" max="11"/>
-    <col width="17.8984375" bestFit="1" customWidth="1" style="20" min="12" max="12"/>
-    <col width="13.5" bestFit="1" customWidth="1" style="20" min="13" max="13"/>
-    <col width="14.296875" bestFit="1" customWidth="1" style="20" min="14" max="14"/>
-    <col width="14" bestFit="1" customWidth="1" style="20" min="15" max="15"/>
-    <col width="16.296875" bestFit="1" customWidth="1" style="20" min="16" max="16"/>
-    <col width="24.59765625" bestFit="1" customWidth="1" style="20" min="17" max="17"/>
-    <col width="31.5" bestFit="1" customWidth="1" style="20" min="18" max="18"/>
-    <col width="30.69921875" bestFit="1" customWidth="1" style="20" min="19" max="19"/>
-    <col width="31.796875" bestFit="1" customWidth="1" style="20" min="20" max="20"/>
-    <col width="15.8984375" bestFit="1" customWidth="1" style="20" min="21" max="21"/>
-    <col width="8.8984375" bestFit="1" customWidth="1" style="20" min="22" max="22"/>
-    <col width="23.09765625" bestFit="1" customWidth="1" style="20" min="23" max="23"/>
-    <col width="45.8984375" customWidth="1" style="20" min="24" max="24"/>
-    <col width="24.296875" bestFit="1" customWidth="1" style="20" min="25" max="25"/>
+    <col width="8.09765625" bestFit="1" customWidth="1" style="21" min="1" max="1"/>
+    <col width="12.09765625" bestFit="1" customWidth="1" style="21" min="2" max="2"/>
+    <col width="9.09765625" bestFit="1" customWidth="1" style="21" min="3" max="3"/>
+    <col width="9.796875" bestFit="1" customWidth="1" style="21" min="4" max="4"/>
+    <col width="18.296875" bestFit="1" customWidth="1" style="21" min="5" max="5"/>
+    <col width="16.19921875" bestFit="1" customWidth="1" style="21" min="6" max="6"/>
+    <col width="15.8984375" bestFit="1" customWidth="1" style="21" min="7" max="7"/>
+    <col width="21.69921875" bestFit="1" customWidth="1" style="21" min="8" max="8"/>
+    <col width="21.59765625" bestFit="1" customWidth="1" style="21" min="9" max="9"/>
+    <col width="11.8984375" bestFit="1" customWidth="1" style="21" min="10" max="10"/>
+    <col width="15.69921875" bestFit="1" customWidth="1" style="21" min="11" max="11"/>
+    <col width="17.8984375" bestFit="1" customWidth="1" style="21" min="12" max="12"/>
+    <col width="13.5" bestFit="1" customWidth="1" style="21" min="13" max="13"/>
+    <col width="14.296875" bestFit="1" customWidth="1" style="21" min="14" max="14"/>
+    <col width="14" bestFit="1" customWidth="1" style="21" min="15" max="15"/>
+    <col width="16.296875" bestFit="1" customWidth="1" style="21" min="16" max="16"/>
+    <col width="24.59765625" bestFit="1" customWidth="1" style="21" min="17" max="17"/>
+    <col width="31.5" bestFit="1" customWidth="1" style="21" min="18" max="18"/>
+    <col width="30.69921875" bestFit="1" customWidth="1" style="21" min="19" max="19"/>
+    <col width="31.796875" bestFit="1" customWidth="1" style="21" min="20" max="20"/>
+    <col width="15.8984375" bestFit="1" customWidth="1" style="21" min="21" max="21"/>
+    <col width="8.8984375" bestFit="1" customWidth="1" style="21" min="22" max="22"/>
+    <col width="23.09765625" bestFit="1" customWidth="1" style="21" min="23" max="23"/>
+    <col width="45.8984375" customWidth="1" style="21" min="24" max="24"/>
+    <col width="24.296875" bestFit="1" customWidth="1" style="21" min="25" max="25"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2" ht="28.8" customFormat="1" customHeight="1" s="1">
+    <row r="2" ht="43.2" customFormat="1" customHeight="1" s="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>VERSION</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>HSR ID</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>SM ID</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>IP NAME</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>IP CLOCK NAME</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>IP RESET NAME</t>
-        </is>
-      </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
+          <t>CLOCK</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>RESET</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
           <t>IP INSTANCE PATH</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
         <is>
           <t>IP SIGNAL PORT NAME</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>IP PARITY PORT NAME</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>IP FILE LIST</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="K2" s="1" t="inlineStr">
         <is>
           <t>IP ERROR PORT</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>IP ERROR DOUBLE</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>BIT WIDTH</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>PARITY SOURCE BIT WIDTH</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>FAULT INJECTION</t>
         </is>
       </c>
-      <c r="N2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>FAULT INJECTION LOCATION</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>EVEN ODD</t>
         </is>
       </c>
-      <c r="P2" s="1" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>NOTE</t>
         </is>
       </c>
     </row>
     <row r="3" ht="28.8" customFormat="1" customHeight="1" s="1">
-      <c r="B3" s="1" t="inlineStr">
+      <c r="D3" s="1" t="inlineStr">
         <is>
           <t>BOS_AXICRYPT</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>I_CLK</t>
         </is>
       </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="F3" s="1" t="inlineStr">
         <is>
           <t>I_RESETN</t>
         </is>
       </c>
-      <c r="F3" s="1" t="inlineStr">
+      <c r="H3" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_ARADDR</t>
         </is>
       </c>
-      <c r="G3" s="1" t="inlineStr">
+      <c r="I3" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_ARADDR_PARITY</t>
         </is>
       </c>
-      <c r="H3" s="1" t="inlineStr">
+      <c r="J3" s="1" t="inlineStr">
         <is>
           <t>$AXICRYPT_HOME/RTL/filelist.f</t>
         </is>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="M3" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="N3" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="M3" s="1" t="inlineStr">
+      <c r="O3" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_ARADDR[0]@FIERR_AXICRYPT_AXI_MI0_ARADDR_PARITY</t>
         </is>
       </c>
-      <c r="O3" s="1" t="inlineStr">
+      <c r="Q3" s="1" t="inlineStr">
         <is>
           <t>EVEN</t>
         </is>
       </c>
     </row>
     <row r="4" ht="28.8" customFormat="1" customHeight="1" s="1">
-      <c r="B4" s="1" t="inlineStr">
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>BOS_AXICRYPT</t>
         </is>
       </c>
-      <c r="C4" s="1" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>I_CLK</t>
         </is>
       </c>
-      <c r="D4" s="1" t="inlineStr">
+      <c r="F4" s="1" t="inlineStr">
         <is>
           <t>I_RESETN</t>
         </is>
       </c>
-      <c r="F4" s="1" t="inlineStr">
+      <c r="H4" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_AWADDR</t>
         </is>
       </c>
-      <c r="G4" s="1" t="inlineStr">
+      <c r="I4" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_AWADDR_PARITY</t>
         </is>
       </c>
-      <c r="H4" s="1" t="inlineStr">
+      <c r="J4" s="1" t="inlineStr">
         <is>
           <t>$AXICRYPT_HOME/RTL/filelist.f</t>
         </is>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="M4" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="L4" s="1" t="n">
+      <c r="N4" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="M4" s="1" t="inlineStr">
+      <c r="O4" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_AWADDR[0]@FIERR_AXICRYPT_AXI_MI0_AWADDR_PARITY</t>
         </is>
       </c>
-      <c r="O4" s="1" t="inlineStr">
+      <c r="Q4" s="1" t="inlineStr">
         <is>
           <t>EVEN</t>
         </is>
       </c>
     </row>
-    <row r="5" customFormat="1" s="1">
-      <c r="B5" s="1" t="inlineStr">
+    <row r="5" ht="28.8" customFormat="1" customHeight="1" s="1">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>BOS_AXICRYPT</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>I_CLK</t>
         </is>
       </c>
-      <c r="D5" s="1" t="inlineStr">
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>I_RESETN</t>
         </is>
       </c>
-      <c r="F5" s="1" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_RDATA</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
+      <c r="I5" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_RDATA_PARITY</t>
         </is>
       </c>
-      <c r="H5" s="1" t="inlineStr">
+      <c r="J5" s="1" t="inlineStr">
         <is>
           <t>$AXICRYPT_HOME/RTL/filelist.f</t>
         </is>
       </c>
-      <c r="I5" s="1" t="inlineStr">
+      <c r="K5" s="1" t="inlineStr">
         <is>
           <t>ERR_AXICRYPT_AXI_MI0_BUS_PARITY</t>
         </is>
       </c>
-      <c r="J5" s="1" t="inlineStr">
+      <c r="L5" s="1" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="M5" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="N5" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="O5" s="1" t="inlineStr">
+      <c r="Q5" s="1" t="inlineStr">
         <is>
           <t>EVEN</t>
         </is>
       </c>
     </row>
     <row r="6" ht="57.6" customFormat="1" customHeight="1" s="1">
-      <c r="B6" s="1" t="inlineStr">
+      <c r="D6" s="1" t="inlineStr">
         <is>
           <t>BOS_AXICRYPT</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
+      <c r="E6" s="1" t="inlineStr">
         <is>
           <t>I_CLK</t>
         </is>
       </c>
-      <c r="D6" s="1" t="inlineStr">
+      <c r="F6" s="1" t="inlineStr">
         <is>
           <t>I_RESETN</t>
         </is>
       </c>
-      <c r="F6" s="1" t="inlineStr">
+      <c r="H6" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_WDATA</t>
         </is>
       </c>
-      <c r="G6" s="1" t="inlineStr">
+      <c r="I6" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_WDATA_PARITY</t>
         </is>
       </c>
-      <c r="H6" s="1" t="inlineStr">
+      <c r="J6" s="1" t="inlineStr">
         <is>
           <t>$AXICRYPT_HOME/RTL/filelist.f</t>
         </is>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="M6" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="N6" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="M6" s="1" t="inlineStr">
+      <c r="O6" s="1" t="inlineStr">
         <is>
           <t>AXICRYPT_AXI_MI0_WDATA[0]@FIERR_AXICRYPT_AXI_MI0_WDATA_PARITY[0], AXICRYPT_AXI_MI0_WDATA[128]@FIERR_AXICRYPT_AXI_MI0_WDATA_PARITY[1]</t>
         </is>
       </c>
-      <c r="O6" s="1" t="inlineStr">
+      <c r="Q6" s="1" t="inlineStr">
         <is>
           <t>EVEN</t>
         </is>
@@ -1129,9 +1132,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="19" bestFit="1" customWidth="1" style="20" min="2" max="2"/>
-    <col width="11.09765625" bestFit="1" customWidth="1" style="20" min="4" max="4"/>
-    <col width="21.8984375" bestFit="1" customWidth="1" style="20" min="6" max="6"/>
+    <col width="19" bestFit="1" customWidth="1" style="21" min="2" max="2"/>
+    <col width="11.09765625" bestFit="1" customWidth="1" style="21" min="4" max="4"/>
+    <col width="21.8984375" bestFit="1" customWidth="1" style="21" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1241,11 +1244,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="21.09765625" bestFit="1" customWidth="1" style="20" min="2" max="2"/>
-    <col width="31.59765625" bestFit="1" customWidth="1" style="20" min="3" max="3"/>
-    <col width="7.8984375" bestFit="1" customWidth="1" style="20" min="4" max="4"/>
-    <col width="43.5" customWidth="1" style="20" min="5" max="5"/>
-    <col width="62.8984375" customWidth="1" style="20" min="7" max="7"/>
+    <col width="21.09765625" bestFit="1" customWidth="1" style="21" min="2" max="2"/>
+    <col width="31.59765625" bestFit="1" customWidth="1" style="21" min="3" max="3"/>
+    <col width="7.8984375" bestFit="1" customWidth="1" style="21" min="4" max="4"/>
+    <col width="43.5" customWidth="1" style="21" min="5" max="5"/>
+    <col width="62.8984375" customWidth="1" style="21" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1292,7 +1295,7 @@
       <c r="F3" s="7" t="n"/>
       <c r="G3" s="7" t="n"/>
     </row>
-    <row r="4" ht="41.4" customHeight="1" s="20">
+    <row r="4" ht="41.4" customHeight="1" s="21">
       <c r="B4" s="6" t="n"/>
       <c r="C4" s="6" t="inlineStr">
         <is>
@@ -1311,12 +1314,12 @@
     </row>
     <row r="5">
       <c r="B5" s="6" t="n"/>
-      <c r="C5" s="19" t="inlineStr">
+      <c r="C5" s="20" t="inlineStr">
         <is>
           <t>VERSION</t>
         </is>
       </c>
-      <c r="D5" s="19" t="n"/>
+      <c r="D5" s="20" t="n"/>
       <c r="E5" s="13" t="inlineStr">
         <is>
           <t>- Version of parameters in the row.</t>
@@ -1335,12 +1338,12 @@
     </row>
     <row r="6">
       <c r="B6" s="6" t="n"/>
-      <c r="C6" s="19" t="inlineStr">
+      <c r="C6" s="20" t="inlineStr">
         <is>
           <t>HSR ID</t>
         </is>
       </c>
-      <c r="D6" s="19" t="n">
+      <c r="D6" s="20" t="n">
         <v>3</v>
       </c>
       <c r="E6" s="13" t="inlineStr">
@@ -1361,12 +1364,12 @@
     </row>
     <row r="7">
       <c r="B7" s="6" t="n"/>
-      <c r="C7" s="19" t="inlineStr">
+      <c r="C7" s="20" t="inlineStr">
         <is>
           <t>SM ID</t>
         </is>
       </c>
-      <c r="D7" s="19" t="n">
+      <c r="D7" s="20" t="n">
         <v>3</v>
       </c>
       <c r="E7" s="13" t="inlineStr">
@@ -1385,14 +1388,14 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="27.6" customHeight="1" s="20">
+    <row r="8" ht="27.6" customHeight="1" s="21">
       <c r="B8" s="6" t="n"/>
       <c r="C8" s="10" t="inlineStr">
         <is>
           <t>BLOCK NAME</t>
         </is>
       </c>
-      <c r="D8" s="19" t="n"/>
+      <c r="D8" s="20" t="n"/>
       <c r="E8" s="9" t="inlineStr">
         <is>
           <t>Block name of the target instance. Target instance is the instance that will be duplicated.</t>
@@ -1407,12 +1410,12 @@
     </row>
     <row r="9">
       <c r="B9" s="6" t="n"/>
-      <c r="C9" s="19" t="inlineStr">
+      <c r="C9" s="20" t="inlineStr">
         <is>
           <t>IP NAME</t>
         </is>
       </c>
-      <c r="D9" s="19" t="n"/>
+      <c r="D9" s="20" t="n"/>
       <c r="E9" s="13" t="inlineStr">
         <is>
           <t>- On-boarding IP’s module name of the target instance.</t>
@@ -1429,14 +1432,14 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="27.6" customHeight="1" s="20">
+    <row r="10" ht="27.6" customHeight="1" s="21">
       <c r="B10" s="6" t="n"/>
       <c r="C10" s="10" t="inlineStr">
         <is>
           <t>TARGET ERROR COLLECTOR</t>
         </is>
       </c>
-      <c r="D10" s="19" t="n"/>
+      <c r="D10" s="20" t="n"/>
       <c r="E10" s="9" t="inlineStr">
         <is>
           <t>The error collector module that receives the error and generates the related fault injection and others.</t>
@@ -1449,14 +1452,14 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="27.6" customHeight="1" s="20">
+    <row r="11" ht="27.6" customHeight="1" s="21">
       <c r="B11" s="6" t="n"/>
       <c r="C11" s="10" t="inlineStr">
         <is>
           <t>IP INSTANCE PATH</t>
         </is>
       </c>
-      <c r="D11" s="19" t="n"/>
+      <c r="D11" s="20" t="n"/>
       <c r="E11" s="9" t="inlineStr">
         <is>
           <t>The &lt;IP NAME&gt; instance path from the &lt;BLOCK NAME&gt;.</t>
@@ -1469,14 +1472,14 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="27.6" customHeight="1" s="20">
+    <row r="12" ht="27.6" customHeight="1" s="21">
       <c r="B12" s="6" t="n"/>
-      <c r="C12" s="19" t="inlineStr">
+      <c r="C12" s="20" t="inlineStr">
         <is>
           <t>TARGET MODULE</t>
         </is>
       </c>
-      <c r="D12" s="19" t="n"/>
+      <c r="D12" s="20" t="n"/>
       <c r="E12" s="13" t="inlineStr">
         <is>
           <t>- The name of the duplicated module.
@@ -1490,14 +1493,14 @@
       </c>
       <c r="G12" s="12" t="n"/>
     </row>
-    <row r="13" ht="41.4" customHeight="1" s="20">
+    <row r="13" ht="41.4" customHeight="1" s="21">
       <c r="B13" s="6" t="n"/>
-      <c r="C13" s="19" t="inlineStr">
+      <c r="C13" s="20" t="inlineStr">
         <is>
           <t>TARGET FILE PATH</t>
         </is>
       </c>
-      <c r="D13" s="19" t="n"/>
+      <c r="D13" s="20" t="n"/>
       <c r="E13" s="13" t="inlineStr">
         <is>
           <t>- The name of the file which contains the duplicated module.
@@ -1511,14 +1514,14 @@
       </c>
       <c r="G13" s="7" t="n"/>
     </row>
-    <row r="14" ht="41.4" customHeight="1" s="20">
+    <row r="14" ht="41.4" customHeight="1" s="21">
       <c r="B14" s="6" t="n"/>
-      <c r="C14" s="19" t="inlineStr">
+      <c r="C14" s="20" t="inlineStr">
         <is>
           <t>TARGET INSTANCE PATH</t>
         </is>
       </c>
-      <c r="D14" s="19" t="n"/>
+      <c r="D14" s="20" t="n"/>
       <c r="E14" s="13" t="inlineStr">
         <is>
           <t>- The target's instance path from IP level before dupication
@@ -1538,12 +1541,12 @@
     </row>
     <row r="15">
       <c r="B15" s="6" t="n"/>
-      <c r="C15" s="19" t="inlineStr">
+      <c r="C15" s="20" t="inlineStr">
         <is>
           <t>OUTPUT LOCATION</t>
         </is>
       </c>
-      <c r="D15" s="19" t="n"/>
+      <c r="D15" s="20" t="n"/>
       <c r="E15" s="13" t="inlineStr">
         <is>
           <t>- Ex) $AXICRYPT_HOME/RTL/SAFETY</t>
@@ -1552,14 +1555,14 @@
       <c r="F15" s="9" t="n"/>
       <c r="G15" s="7" t="n"/>
     </row>
-    <row r="16" ht="69" customHeight="1" s="20">
+    <row r="16" ht="69" customHeight="1" s="21">
       <c r="B16" s="6" t="n"/>
-      <c r="C16" s="19" t="inlineStr">
+      <c r="C16" s="20" t="inlineStr">
         <is>
           <t>OUTPUT INSTANCE PATH</t>
         </is>
       </c>
-      <c r="D16" s="19" t="inlineStr">
+      <c r="D16" s="20" t="inlineStr">
         <is>
           <t>V3.0</t>
         </is>
@@ -1581,14 +1584,14 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="82.8" customHeight="1" s="20">
+    <row r="17" ht="82.8" customHeight="1" s="21">
       <c r="B17" s="6" t="n"/>
-      <c r="C17" s="19" t="inlineStr">
+      <c r="C17" s="20" t="inlineStr">
         <is>
           <t>DUPLICATED OUTPUT INSTANCE PATH</t>
         </is>
       </c>
-      <c r="D17" s="19" t="inlineStr">
+      <c r="D17" s="20" t="inlineStr">
         <is>
           <t>V3.0</t>
         </is>
@@ -1610,14 +1613,14 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="151.8" customHeight="1" s="20">
+    <row r="18" ht="151.8" customHeight="1" s="21">
       <c r="B18" s="6" t="n"/>
       <c r="C18" s="10" t="inlineStr">
         <is>
           <t>DUPLICATION TYPE</t>
         </is>
       </c>
-      <c r="D18" s="19" t="n"/>
+      <c r="D18" s="20" t="n"/>
       <c r="E18" s="13" t="inlineStr">
         <is>
           <t>- WRAP or FLAT (WRAP type only supported).
@@ -1638,12 +1641,12 @@
     </row>
     <row r="19">
       <c r="B19" s="6" t="n"/>
-      <c r="C19" s="19" t="inlineStr">
+      <c r="C19" s="20" t="inlineStr">
         <is>
           <t>DCLS ERROR OUTPUT PORT</t>
         </is>
       </c>
-      <c r="D19" s="19" t="n"/>
+      <c r="D19" s="20" t="n"/>
       <c r="E19" s="9" t="inlineStr">
         <is>
           <t>Error signal port name at IP top level</t>
@@ -1660,14 +1663,14 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="41.4" customHeight="1" s="20">
+    <row r="20" ht="41.4" customHeight="1" s="21">
       <c r="B20" s="6" t="n"/>
-      <c r="C20" s="19" t="inlineStr">
+      <c r="C20" s="20" t="inlineStr">
         <is>
           <t>DCLS ERROR DOUBLE</t>
         </is>
       </c>
-      <c r="D20" s="19" t="n"/>
+      <c r="D20" s="20" t="n"/>
       <c r="E20" s="13" t="inlineStr">
         <is>
           <t>- YES or NO.
@@ -1683,12 +1686,12 @@
     </row>
     <row r="21">
       <c r="B21" s="6" t="n"/>
-      <c r="C21" s="19" t="inlineStr">
+      <c r="C21" s="20" t="inlineStr">
         <is>
           <t>CLOCK</t>
         </is>
       </c>
-      <c r="D21" s="19" t="n"/>
+      <c r="D21" s="20" t="n"/>
       <c r="E21" s="9" t="inlineStr">
         <is>
           <t>The clock port name used in the duplicated module</t>
@@ -1707,12 +1710,12 @@
     </row>
     <row r="22">
       <c r="B22" s="6" t="n"/>
-      <c r="C22" s="19" t="inlineStr">
+      <c r="C22" s="20" t="inlineStr">
         <is>
           <t>RESET</t>
         </is>
       </c>
-      <c r="D22" s="19" t="n"/>
+      <c r="D22" s="20" t="n"/>
       <c r="E22" s="9" t="inlineStr">
         <is>
           <t>The reset port name used in the duplicated module</t>
@@ -1729,14 +1732,14 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="41.4" customHeight="1" s="20">
+    <row r="23" ht="41.4" customHeight="1" s="21">
       <c r="B23" s="6" t="n"/>
       <c r="C23" s="10" t="inlineStr">
         <is>
           <t>RESET_2D</t>
         </is>
       </c>
-      <c r="D23" s="19" t="n"/>
+      <c r="D23" s="20" t="n"/>
       <c r="E23" s="9" t="inlineStr">
         <is>
           <t>The 2-cycle delayed reset port name used in the duplicated module. This reset signal is needed if the IP starts operations after reset is de-asserted.</t>
@@ -1749,14 +1752,14 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="69" customHeight="1" s="20">
+    <row r="24" ht="69" customHeight="1" s="21">
       <c r="B24" s="6" t="n"/>
-      <c r="C24" s="19" t="inlineStr">
+      <c r="C24" s="20" t="inlineStr">
         <is>
           <t>IGNORE INPUT</t>
         </is>
       </c>
-      <c r="D24" s="19" t="n"/>
+      <c r="D24" s="20" t="n"/>
       <c r="E24" s="13" t="inlineStr">
         <is>
           <t>- These signals are supplied to the original and the duplicated module without 2-cycle delay.
@@ -1771,14 +1774,14 @@
       </c>
       <c r="G24" s="7" t="n"/>
     </row>
-    <row r="25" ht="41.4" customHeight="1" s="20">
+    <row r="25" ht="41.4" customHeight="1" s="21">
       <c r="B25" s="6" t="n"/>
-      <c r="C25" s="19" t="inlineStr">
+      <c r="C25" s="20" t="inlineStr">
         <is>
           <t>IGNORE OUTPUT</t>
         </is>
       </c>
-      <c r="D25" s="19" t="n"/>
+      <c r="D25" s="20" t="n"/>
       <c r="E25" s="13" t="inlineStr">
         <is>
           <t>- The ignored output that are not compared. Analog or other clock domain can be ignored.
@@ -1792,14 +1795,14 @@
       </c>
       <c r="G25" s="7" t="n"/>
     </row>
-    <row r="26" ht="179.4" customHeight="1" s="20">
+    <row r="26" ht="179.4" customHeight="1" s="21">
       <c r="B26" s="6" t="n"/>
-      <c r="C26" s="19" t="inlineStr">
+      <c r="C26" s="20" t="inlineStr">
         <is>
           <t>INPUT VALID</t>
         </is>
       </c>
-      <c r="D26" s="19" t="n"/>
+      <c r="D26" s="20" t="n"/>
       <c r="E26" s="13" t="inlineStr">
         <is>
           <t>- The input is applied to the duplicated core when the &lt;INPUT VALID&gt; is high or low. The final condition is Ored.
@@ -1815,14 +1818,14 @@
       </c>
       <c r="G26" s="7" t="n"/>
     </row>
-    <row r="27" ht="124.2" customHeight="1" s="20">
+    <row r="27" ht="124.2" customHeight="1" s="21">
       <c r="B27" s="6" t="n"/>
-      <c r="C27" s="19" t="inlineStr">
+      <c r="C27" s="20" t="inlineStr">
         <is>
           <t>OUTPUT VALID</t>
         </is>
       </c>
-      <c r="D27" s="19" t="n"/>
+      <c r="D27" s="20" t="n"/>
       <c r="E27" s="13" t="inlineStr">
         <is>
           <t>- The output is compared when the &lt;OUTPUT VALID&gt; is high or low. The final condition is Ored.
@@ -1838,14 +1841,14 @@
       </c>
       <c r="G27" s="7" t="n"/>
     </row>
-    <row r="28" ht="69" customHeight="1" s="20">
+    <row r="28" ht="69" customHeight="1" s="21">
       <c r="B28" s="6" t="n"/>
-      <c r="C28" s="19" t="inlineStr">
+      <c r="C28" s="20" t="inlineStr">
         <is>
           <t>DEFAULT RESET VALUE</t>
         </is>
       </c>
-      <c r="D28" s="19" t="n"/>
+      <c r="D28" s="20" t="n"/>
       <c r="E28" s="13" t="inlineStr">
         <is>
           <t>- Reset value of a signal (by default, reset value of a signal is 0). There is no issue although the reset value is not correctly set because the first 2 cycle error condition is ignored.
@@ -1861,12 +1864,12 @@
     </row>
     <row r="29">
       <c r="B29" s="6" t="n"/>
-      <c r="C29" s="19" t="inlineStr">
+      <c r="C29" s="20" t="inlineStr">
         <is>
           <t>DESIGN FILE LIST</t>
         </is>
       </c>
-      <c r="D29" s="19" t="n"/>
+      <c r="D29" s="20" t="n"/>
       <c r="E29" s="13" t="inlineStr">
         <is>
           <t>- Design file list for the duplication script</t>
@@ -1883,14 +1886,14 @@
         </is>
       </c>
     </row>
-    <row r="30" ht="55.2" customHeight="1" s="20">
+    <row r="30" ht="55.2" customHeight="1" s="21">
       <c r="B30" s="6" t="n"/>
       <c r="C30" s="14" t="inlineStr">
         <is>
           <t>FAULT INJECTION PORT</t>
         </is>
       </c>
-      <c r="D30" s="19" t="n"/>
+      <c r="D30" s="20" t="n"/>
       <c r="E30" s="13" t="inlineStr">
         <is>
           <t>- The fault injection port name is FI&lt;IP ERROR PORT&gt; in default. @&lt;Fault Injection Port&gt; can be described and it just means the fault injection port name only.
@@ -1916,7 +1919,7 @@
           <t>COMPARATOR INPUT WIDTH</t>
         </is>
       </c>
-      <c r="D31" s="19" t="inlineStr">
+      <c r="D31" s="20" t="inlineStr">
         <is>
           <t>V3.0</t>
         </is>
@@ -1929,14 +1932,14 @@
       </c>
       <c r="G31" s="7" t="n"/>
     </row>
-    <row r="32" ht="82.8" customHeight="1" s="20">
+    <row r="32" ht="82.8" customHeight="1" s="21">
       <c r="B32" s="6" t="n"/>
       <c r="C32" s="15" t="inlineStr">
         <is>
           <t>COMPARATOR DEPTH</t>
         </is>
       </c>
-      <c r="D32" s="19" t="inlineStr">
+      <c r="D32" s="20" t="inlineStr">
         <is>
           <t>V3.0</t>
         </is>
@@ -1960,12 +1963,12 @@
     </row>
     <row r="33">
       <c r="B33" s="6" t="n"/>
-      <c r="C33" s="19" t="inlineStr">
+      <c r="C33" s="20" t="inlineStr">
         <is>
           <t>NOTE</t>
         </is>
       </c>
-      <c r="D33" s="19" t="n"/>
+      <c r="D33" s="20" t="n"/>
       <c r="E33" s="9" t="inlineStr">
         <is>
           <t>Note description</t>
@@ -1992,12 +1995,12 @@
     </row>
     <row r="35">
       <c r="B35" s="6" t="n"/>
-      <c r="C35" s="19" t="inlineStr">
+      <c r="C35" s="20" t="inlineStr">
         <is>
           <t>VERSION</t>
         </is>
       </c>
-      <c r="D35" s="19" t="n"/>
+      <c r="D35" s="20" t="n"/>
       <c r="E35" s="9" t="inlineStr">
         <is>
           <t>Version number of the parameters for Safety Mechanism</t>
@@ -2008,12 +2011,12 @@
     </row>
     <row r="36">
       <c r="B36" s="6" t="n"/>
-      <c r="C36" s="19" t="inlineStr">
+      <c r="C36" s="20" t="inlineStr">
         <is>
           <t>HSR ID</t>
         </is>
       </c>
-      <c r="D36" s="19" t="n"/>
+      <c r="D36" s="20" t="n"/>
       <c r="E36" s="9" t="inlineStr">
         <is>
           <t>Corresponding HSR ID for this INFO file</t>
@@ -2024,12 +2027,12 @@
     </row>
     <row r="37">
       <c r="B37" s="6" t="n"/>
-      <c r="C37" s="19" t="inlineStr">
+      <c r="C37" s="20" t="inlineStr">
         <is>
           <t>SM ID</t>
         </is>
       </c>
-      <c r="D37" s="19" t="n"/>
+      <c r="D37" s="20" t="n"/>
       <c r="E37" s="9" t="inlineStr">
         <is>
           <t>Safety mechanism ID</t>
@@ -2040,12 +2043,12 @@
     </row>
     <row r="38">
       <c r="B38" s="6" t="n"/>
-      <c r="C38" s="19" t="inlineStr">
+      <c r="C38" s="20" t="inlineStr">
         <is>
           <t>BLOCK NAME</t>
         </is>
       </c>
-      <c r="D38" s="19" t="n"/>
+      <c r="D38" s="20" t="n"/>
       <c r="E38" s="9" t="inlineStr">
         <is>
           <t>Block name of the target instance</t>
@@ -2054,14 +2057,14 @@
       <c r="F38" s="9" t="n"/>
       <c r="G38" s="7" t="n"/>
     </row>
-    <row r="39" ht="82.8" customHeight="1" s="20">
+    <row r="39" ht="82.8" customHeight="1" s="21">
       <c r="B39" s="6" t="n"/>
-      <c r="C39" s="19" t="inlineStr">
+      <c r="C39" s="20" t="inlineStr">
         <is>
           <t>BUS TYPE</t>
         </is>
       </c>
-      <c r="D39" s="19" t="n"/>
+      <c r="D39" s="20" t="n"/>
       <c r="E39" s="9" t="inlineStr">
         <is>
           <t>MST, SLV, MST_IF, SLV_IF types are available. MST is master type from IP side. SLV is slave type from IP side. MST_IF is bus interface type from master IP. SLV_IF is bus interface type from slave IP. Interface type means the bus is connected between IPs and the IP is the master.</t>
@@ -2072,12 +2075,12 @@
     </row>
     <row r="40">
       <c r="B40" s="6" t="n"/>
-      <c r="C40" s="19" t="inlineStr">
+      <c r="C40" s="20" t="inlineStr">
         <is>
           <t>BUS NAME</t>
         </is>
       </c>
-      <c r="D40" s="19" t="n"/>
+      <c r="D40" s="20" t="n"/>
       <c r="E40" s="9" t="inlineStr">
         <is>
           <t>BUS module name of &lt;BUS INSTANCE PATH&gt;</t>
@@ -2088,12 +2091,12 @@
     </row>
     <row r="41">
       <c r="B41" s="6" t="n"/>
-      <c r="C41" s="19" t="inlineStr">
+      <c r="C41" s="20" t="inlineStr">
         <is>
           <t>BUS INSTANCE PATH</t>
         </is>
       </c>
-      <c r="D41" s="19" t="n"/>
+      <c r="D41" s="20" t="n"/>
       <c r="E41" s="9" t="inlineStr">
         <is>
           <t>BUS module instance path in the &lt;BLOCK NAME&gt;</t>
@@ -2104,36 +2107,36 @@
     </row>
     <row r="42">
       <c r="B42" s="6" t="n"/>
-      <c r="C42" s="19" t="inlineStr">
+      <c r="C42" s="20" t="inlineStr">
         <is>
           <t>BUS CLOCK NAME</t>
         </is>
       </c>
-      <c r="D42" s="19" t="n"/>
+      <c r="D42" s="20" t="n"/>
       <c r="E42" s="9" t="n"/>
       <c r="F42" s="9" t="n"/>
       <c r="G42" s="7" t="n"/>
     </row>
     <row r="43">
       <c r="B43" s="6" t="n"/>
-      <c r="C43" s="19" t="inlineStr">
+      <c r="C43" s="20" t="inlineStr">
         <is>
           <t>BUS RESET NAME</t>
         </is>
       </c>
-      <c r="D43" s="19" t="n"/>
+      <c r="D43" s="20" t="n"/>
       <c r="E43" s="9" t="n"/>
       <c r="F43" s="9" t="n"/>
       <c r="G43" s="7" t="n"/>
     </row>
-    <row r="44" ht="27.6" customHeight="1" s="20">
+    <row r="44" ht="27.6" customHeight="1" s="21">
       <c r="B44" s="6" t="n"/>
-      <c r="C44" s="19" t="inlineStr">
+      <c r="C44" s="20" t="inlineStr">
         <is>
           <t>BUS SIGNAL PORT NAME</t>
         </is>
       </c>
-      <c r="D44" s="19" t="n"/>
+      <c r="D44" s="20" t="n"/>
       <c r="E44" s="9" t="inlineStr">
         <is>
           <t>Target bus port names in &lt;BUS INSTANCE PATH&gt; for the bus parity.</t>
@@ -2142,14 +2145,14 @@
       <c r="F44" s="9" t="n"/>
       <c r="G44" s="7" t="n"/>
     </row>
-    <row r="45" ht="41.4" customHeight="1" s="20">
+    <row r="45" ht="41.4" customHeight="1" s="21">
       <c r="B45" s="6" t="n"/>
-      <c r="C45" s="19" t="inlineStr">
+      <c r="C45" s="20" t="inlineStr">
         <is>
           <t>BUS SIGNAL VALID</t>
         </is>
       </c>
-      <c r="D45" s="19" t="n"/>
+      <c r="D45" s="20" t="n"/>
       <c r="E45" s="9" t="inlineStr">
         <is>
           <t>&lt;BUS SIGNAL PORT NAME&gt;’s parity is checked when &lt;BUS SIGNAL VALID&gt; condition. If not specified, always checked</t>
@@ -2160,12 +2163,12 @@
     </row>
     <row r="46">
       <c r="B46" s="6" t="n"/>
-      <c r="C46" s="19" t="inlineStr">
+      <c r="C46" s="20" t="inlineStr">
         <is>
           <t>BUS PARITY PORT NAME</t>
         </is>
       </c>
-      <c r="D46" s="19" t="n"/>
+      <c r="D46" s="20" t="n"/>
       <c r="E46" s="9" t="inlineStr">
         <is>
           <t>The parity port name at BUS side</t>
@@ -2174,14 +2177,14 @@
       <c r="F46" s="9" t="n"/>
       <c r="G46" s="7" t="n"/>
     </row>
-    <row r="47" ht="27.6" customHeight="1" s="20">
+    <row r="47" ht="27.6" customHeight="1" s="21">
       <c r="B47" s="6" t="n"/>
-      <c r="C47" s="19" t="inlineStr">
+      <c r="C47" s="20" t="inlineStr">
         <is>
           <t>BUS FILE LIST</t>
         </is>
       </c>
-      <c r="D47" s="19" t="n"/>
+      <c r="D47" s="20" t="n"/>
       <c r="E47" s="9" t="inlineStr">
         <is>
           <t>The filelist for the bus design. This file can be used to insert the safety mechanism</t>
@@ -2192,12 +2195,12 @@
     </row>
     <row r="48">
       <c r="B48" s="6" t="n"/>
-      <c r="C48" s="19" t="inlineStr">
+      <c r="C48" s="20" t="inlineStr">
         <is>
           <t>BUS ERROR PORT</t>
         </is>
       </c>
-      <c r="D48" s="19" t="n"/>
+      <c r="D48" s="20" t="n"/>
       <c r="E48" s="9" t="inlineStr">
         <is>
           <t>Error signal port name from &lt;BUS INSTANCE PATH&gt;</t>
@@ -2208,12 +2211,12 @@
     </row>
     <row r="49">
       <c r="B49" s="6" t="n"/>
-      <c r="C49" s="19" t="inlineStr">
+      <c r="C49" s="20" t="inlineStr">
         <is>
           <t>BUS ERROR DOUBLE</t>
         </is>
       </c>
-      <c r="D49" s="19" t="n"/>
+      <c r="D49" s="20" t="n"/>
       <c r="E49" s="11" t="inlineStr">
         <is>
           <t>YES or NO. Error signal is doubled if YES</t>
@@ -2240,12 +2243,12 @@
     </row>
     <row r="52">
       <c r="B52" s="6" t="n"/>
-      <c r="C52" s="19" t="inlineStr">
+      <c r="C52" s="20" t="inlineStr">
         <is>
           <t>IP NAME</t>
         </is>
       </c>
-      <c r="D52" s="19" t="n"/>
+      <c r="D52" s="20" t="n"/>
       <c r="E52" s="9" t="inlineStr">
         <is>
           <t>Module name of the target instance</t>
@@ -2256,36 +2259,36 @@
     </row>
     <row r="53">
       <c r="B53" s="6" t="n"/>
-      <c r="C53" s="19" t="inlineStr">
+      <c r="C53" s="20" t="inlineStr">
         <is>
           <t>IP CLOCK NAME</t>
         </is>
       </c>
-      <c r="D53" s="19" t="n"/>
+      <c r="D53" s="20" t="n"/>
       <c r="E53" s="9" t="n"/>
       <c r="F53" s="9" t="n"/>
       <c r="G53" s="7" t="n"/>
     </row>
     <row r="54">
       <c r="B54" s="6" t="n"/>
-      <c r="C54" s="19" t="inlineStr">
+      <c r="C54" s="20" t="inlineStr">
         <is>
           <t>IP RESET NAME</t>
         </is>
       </c>
-      <c r="D54" s="19" t="n"/>
+      <c r="D54" s="20" t="n"/>
       <c r="E54" s="9" t="n"/>
       <c r="F54" s="9" t="n"/>
       <c r="G54" s="7" t="n"/>
     </row>
     <row r="55">
       <c r="B55" s="6" t="n"/>
-      <c r="C55" s="19" t="inlineStr">
+      <c r="C55" s="20" t="inlineStr">
         <is>
           <t>IP INSTANCE PATH</t>
         </is>
       </c>
-      <c r="D55" s="19" t="n"/>
+      <c r="D55" s="20" t="n"/>
       <c r="E55" s="9" t="inlineStr">
         <is>
           <t>IP instance path in the &lt;BLOCK NAME&gt;</t>
@@ -2294,14 +2297,14 @@
       <c r="F55" s="9" t="n"/>
       <c r="G55" s="7" t="n"/>
     </row>
-    <row r="56" ht="27.6" customHeight="1" s="20">
+    <row r="56" ht="27.6" customHeight="1" s="21">
       <c r="B56" s="6" t="n"/>
-      <c r="C56" s="19" t="inlineStr">
+      <c r="C56" s="20" t="inlineStr">
         <is>
           <t>IP SIGNAL PORT NAME</t>
         </is>
       </c>
-      <c r="D56" s="19" t="n"/>
+      <c r="D56" s="20" t="n"/>
       <c r="E56" s="9" t="inlineStr">
         <is>
           <t>Target bus port names in &lt;IP INSTANCE PATH&gt; for the bus parity</t>
@@ -2310,14 +2313,14 @@
       <c r="F56" s="9" t="n"/>
       <c r="G56" s="7" t="n"/>
     </row>
-    <row r="57" ht="41.4" customHeight="1" s="20">
+    <row r="57" ht="41.4" customHeight="1" s="21">
       <c r="B57" s="6" t="n"/>
-      <c r="C57" s="19" t="inlineStr">
+      <c r="C57" s="20" t="inlineStr">
         <is>
           <t>IP SIGNAL VALID</t>
         </is>
       </c>
-      <c r="D57" s="19" t="n"/>
+      <c r="D57" s="20" t="n"/>
       <c r="E57" s="9" t="inlineStr">
         <is>
           <t>&lt;IP SIGNAL PORT NAME&gt;’s parity is checked when &lt;IP SIGNAL VALID&gt; condition. If not specified, always checked</t>
@@ -2328,12 +2331,12 @@
     </row>
     <row r="58">
       <c r="B58" s="6" t="n"/>
-      <c r="C58" s="19" t="inlineStr">
+      <c r="C58" s="20" t="inlineStr">
         <is>
           <t>IP PARITY PORT NAME</t>
         </is>
       </c>
-      <c r="D58" s="19" t="n"/>
+      <c r="D58" s="20" t="n"/>
       <c r="E58" s="9" t="inlineStr">
         <is>
           <t>The parity port name at IP side</t>
@@ -2342,14 +2345,14 @@
       <c r="F58" s="9" t="n"/>
       <c r="G58" s="7" t="n"/>
     </row>
-    <row r="59" ht="27.6" customHeight="1" s="20">
+    <row r="59" ht="27.6" customHeight="1" s="21">
       <c r="B59" s="6" t="n"/>
-      <c r="C59" s="19" t="inlineStr">
+      <c r="C59" s="20" t="inlineStr">
         <is>
           <t>IP FILE LIST</t>
         </is>
       </c>
-      <c r="D59" s="19" t="n"/>
+      <c r="D59" s="20" t="n"/>
       <c r="E59" s="9" t="inlineStr">
         <is>
           <t>The filelist for the IP design. This file can be used to insert the safety mechanism</t>
@@ -2360,12 +2363,12 @@
     </row>
     <row r="60">
       <c r="B60" s="6" t="n"/>
-      <c r="C60" s="19" t="inlineStr">
+      <c r="C60" s="20" t="inlineStr">
         <is>
           <t>IP ERROR PORT</t>
         </is>
       </c>
-      <c r="D60" s="19" t="n"/>
+      <c r="D60" s="20" t="n"/>
       <c r="E60" s="9" t="inlineStr">
         <is>
           <t>Error signal port name from &lt;IP INSTANCE PATH&gt;</t>
@@ -2376,12 +2379,12 @@
     </row>
     <row r="61">
       <c r="B61" s="6" t="n"/>
-      <c r="C61" s="19" t="inlineStr">
+      <c r="C61" s="20" t="inlineStr">
         <is>
           <t>IP ERROR DOUBLE</t>
         </is>
       </c>
-      <c r="D61" s="19" t="n"/>
+      <c r="D61" s="20" t="n"/>
       <c r="E61" s="11" t="inlineStr">
         <is>
           <t>YES or NO. Error signal is doubled if YES</t>
@@ -2408,12 +2411,12 @@
     </row>
     <row r="64">
       <c r="B64" s="6" t="n"/>
-      <c r="C64" s="19" t="inlineStr">
+      <c r="C64" s="20" t="inlineStr">
         <is>
           <t>BIT WIDTH</t>
         </is>
       </c>
-      <c r="D64" s="19" t="n"/>
+      <c r="D64" s="20" t="n"/>
       <c r="E64" s="9" t="inlineStr">
         <is>
           <t>Bit width of bus port</t>
@@ -2422,14 +2425,14 @@
       <c r="F64" s="9" t="n"/>
       <c r="G64" s="7" t="n"/>
     </row>
-    <row r="65" ht="41.4" customHeight="1" s="20">
+    <row r="65" ht="41.4" customHeight="1" s="21">
       <c r="B65" s="6" t="n"/>
-      <c r="C65" s="19" t="inlineStr">
+      <c r="C65" s="20" t="inlineStr">
         <is>
           <t>PARITY SOURCE BIT WIDTH</t>
         </is>
       </c>
-      <c r="D65" s="19" t="n"/>
+      <c r="D65" s="20" t="n"/>
       <c r="E65" s="9" t="inlineStr">
         <is>
           <t>The bit width that is used to gerenate one parity bit. The number of parity bit is floor (&lt;BIT WIDTH&gt; / &lt;PARITY SOURCE BIT WIDTH&gt;).</t>
@@ -2438,14 +2441,14 @@
       <c r="F65" s="9" t="n"/>
       <c r="G65" s="7" t="n"/>
     </row>
-    <row r="66" ht="41.4" customHeight="1" s="20">
+    <row r="66" ht="41.4" customHeight="1" s="21">
       <c r="B66" s="6" t="n"/>
-      <c r="C66" s="19" t="inlineStr">
+      <c r="C66" s="20" t="inlineStr">
         <is>
           <t>FAULT INJECTION</t>
         </is>
       </c>
-      <c r="D66" s="19" t="n"/>
+      <c r="D66" s="20" t="n"/>
       <c r="E66" s="9" t="inlineStr">
         <is>
           <t>A fault injection port name and the target port to which a fault is injected. The fault injection port name is FI&lt;IP ERROR PORT&gt; in default.</t>
@@ -2460,7 +2463,7 @@
       <c r="F67" s="7" t="n"/>
       <c r="G67" s="7" t="n"/>
     </row>
-    <row r="68" ht="41.4" customHeight="1" s="20">
+    <row r="68" ht="41.4" customHeight="1" s="21">
       <c r="B68" s="6" t="n"/>
       <c r="E68" s="9" t="inlineStr">
         <is>
@@ -2476,7 +2479,7 @@
       <c r="F69" s="7" t="n"/>
       <c r="G69" s="7" t="n"/>
     </row>
-    <row r="70" ht="27.6" customHeight="1" s="20">
+    <row r="70" ht="27.6" customHeight="1" s="21">
       <c r="B70" s="6" t="n"/>
       <c r="E70" s="9" t="inlineStr">
         <is>
@@ -2488,12 +2491,12 @@
     </row>
     <row r="71">
       <c r="B71" s="6" t="n"/>
-      <c r="C71" s="19" t="inlineStr">
+      <c r="C71" s="20" t="inlineStr">
         <is>
           <t>FAULT INJECTION LOCATION</t>
         </is>
       </c>
-      <c r="D71" s="19" t="n"/>
+      <c r="D71" s="20" t="n"/>
       <c r="E71" s="9" t="inlineStr">
         <is>
           <t>The parity checker at the</t>
@@ -2504,12 +2507,12 @@
     </row>
     <row r="72">
       <c r="B72" s="6" t="n"/>
-      <c r="C72" s="19" t="inlineStr">
+      <c r="C72" s="20" t="inlineStr">
         <is>
           <t>EVEN ODD</t>
         </is>
       </c>
-      <c r="D72" s="19" t="n"/>
+      <c r="D72" s="20" t="n"/>
       <c r="E72" s="9" t="inlineStr">
         <is>
           <t>Parity type is specified: EVEN, ODD</t>
@@ -2520,12 +2523,12 @@
     </row>
     <row r="73">
       <c r="B73" s="6" t="n"/>
-      <c r="C73" s="19" t="inlineStr">
+      <c r="C73" s="20" t="inlineStr">
         <is>
           <t>NOTE</t>
         </is>
       </c>
-      <c r="D73" s="19" t="n"/>
+      <c r="D73" s="20" t="n"/>
       <c r="E73" s="9" t="inlineStr">
         <is>
           <t>Note description</t>

</xml_diff>

<commit_message>
Implemented fault injection for parity ganerators
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,15 +516,10 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>FAULT INJECTION LOCATION</t>
+          <t>EVEN ODD</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>EVEN ODD</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>NOTE</t>
         </is>
@@ -572,28 +567,23 @@
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+      <c r="N2" t="n">
+        <v>36</v>
+      </c>
+      <c r="O2" t="n">
+        <v>36</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_ARADDR[0]@FIERR_AXICRYPT_AXI_MI0_ARADDR_PARITY</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr">
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>EVEN</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -637,28 +627,23 @@
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+      <c r="N3" t="n">
+        <v>36</v>
+      </c>
+      <c r="O3" t="n">
+        <v>36</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_AWADDR[0]@FIERR_AXICRYPT_AXI_MI0_AWADDR_PARITY</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>EVEN</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -710,24 +695,23 @@
           <t>YES</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>256</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>128</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr">
+      <c r="N4" t="n">
+        <v>256</v>
+      </c>
+      <c r="O4" t="n">
+        <v>128</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>EVEN</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -771,28 +755,23 @@
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>256</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>128</t>
-        </is>
+      <c r="N5" t="n">
+        <v>256</v>
+      </c>
+      <c r="O5" t="n">
+        <v>128</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_WDATA[0]@FIERR_AXICRYPT_AXI_MI0_WDATA_PARITY[0], AXICRYPT_AXI_MI0_WDATA[128]@FIERR_AXICRYPT_AXI_MI0_WDATA_PARITY[1]</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr">
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>EVEN</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Implemented SIGNAL VALID NAME
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pnson\parity_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02AEC6D-E1B5-411A-95F3-9382CCF84DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB2CE36-1250-4779-A901-12CE61B53C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <t>VERSION</t>
   </si>
@@ -139,7 +139,16 @@
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
+    <t>AXICRYPT_AXI_MI0_ARVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_WVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_RVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_AWVALID</t>
   </si>
 </sst>
 </file>
@@ -505,7 +514,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +522,7 @@
     <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32.6640625" bestFit="1" customWidth="1"/>
@@ -610,6 +619,9 @@
       <c r="I2" t="s">
         <v>24</v>
       </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
       <c r="K2" t="s">
         <v>25</v>
       </c>
@@ -654,6 +666,9 @@
       <c r="I3" t="s">
         <v>24</v>
       </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
       <c r="K3" t="s">
         <v>30</v>
       </c>
@@ -693,10 +708,13 @@
         <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
         <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
       </c>
       <c r="K4" t="s">
         <v>33</v>
@@ -747,6 +765,9 @@
       </c>
       <c r="I5" t="s">
         <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
       </c>
       <c r="K5" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Restore fault injection for receive ports
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pnson\parity_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pnson\Workspace\Parity_Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CA92F3-76D9-402F-A22C-26C198B5DEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF34F6C9-3F7B-49C3-9CE7-0E813DA4BB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAFETY.PARITY" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>VERSION</t>
   </si>
@@ -55,153 +55,159 @@
     <t>IP FILE LIST</t>
   </si>
   <si>
+    <t>ERROR DOUBLE</t>
+  </si>
+  <si>
+    <t>BIT WIDTH</t>
+  </si>
+  <si>
+    <t>PARITY SOURCE BIT WIDTH</t>
+  </si>
+  <si>
+    <t>FAULT INJECTION</t>
+  </si>
+  <si>
+    <t>EVEN ODD</t>
+  </si>
+  <si>
+    <t>COMPARATOR INPUT WIDTH</t>
+  </si>
+  <si>
+    <t>COMPARATOR DEPTH</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>BOS_AXICRYPT</t>
+  </si>
+  <si>
+    <t>I_CLK</t>
+  </si>
+  <si>
+    <t>I_RESETN</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_ARADDR</t>
+  </si>
+  <si>
+    <t>DRIVE</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_ARADDR_PARITY</t>
+  </si>
+  <si>
+    <t>$AXICRYPT_HOME/RTL/filelist.f</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>EVEN</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_AWADDR</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_AWADDR_PARITY</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_RDATA</t>
+  </si>
+  <si>
+    <t>RECEIVE</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_RDATA_PARITY</t>
+  </si>
+  <si>
+    <t>ERR_AXICRYPT_AXI_MI0_BUS_PARITY</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_WDATA</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_WDATA_PARITY</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_AWVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_ARVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_WVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_RVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_MI0_AWVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_ARADDR</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_AWADDR</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_RDATA</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_WDATA</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_ARVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_RVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_WVALID</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_ARADDR_PARITY</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_AWADDR_PARITY</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_RDATA_PARITY</t>
+  </si>
+  <si>
+    <t>AXICRYPT_AXI_SI0_WDATA_PARITY</t>
+  </si>
+  <si>
+    <t>ERR_AXICRYPT_AXI_SI0_BUS_PARITY</t>
+  </si>
+  <si>
+    <t>GROUP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>ERROR PORT</t>
-  </si>
-  <si>
-    <t>ERROR DOUBLE</t>
-  </si>
-  <si>
-    <t>BIT WIDTH</t>
-  </si>
-  <si>
-    <t>PARITY SOURCE BIT WIDTH</t>
-  </si>
-  <si>
-    <t>FAULT INJECTION</t>
-  </si>
-  <si>
-    <t>EVEN ODD</t>
-  </si>
-  <si>
-    <t>COMPARATOR INPUT WIDTH</t>
-  </si>
-  <si>
-    <t>COMPARATOR DEPTH</t>
-  </si>
-  <si>
-    <t>NOTE</t>
-  </si>
-  <si>
-    <t>BOS_AXICRYPT</t>
-  </si>
-  <si>
-    <t>I_CLK</t>
-  </si>
-  <si>
-    <t>I_RESETN</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_ARADDR</t>
-  </si>
-  <si>
-    <t>DRIVE</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_ARADDR_PARITY</t>
-  </si>
-  <si>
-    <t>$AXICRYPT_HOME/RTL/filelist.f</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>EVEN</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_AWADDR</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_AWADDR_PARITY</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_RDATA</t>
-  </si>
-  <si>
-    <t>RECEIVE</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_RDATA_PARITY</t>
-  </si>
-  <si>
-    <t>ERR_AXICRYPT_AXI_MI0_BUS_PARITY</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_WDATA</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_WDATA_PARITY</t>
-  </si>
-  <si>
-    <t>GROUP</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_AWVALID</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_ARVALID</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_WVALID</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_RVALID</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_MI0_AWVALID</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_ARADDR</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_AWADDR</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_RDATA</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_WDATA</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_ARVALID</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_RVALID</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_WVALID</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_ARADDR_PARITY</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_AWADDR_PARITY</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_RDATA_PARITY</t>
-  </si>
-  <si>
-    <t>AXICRYPT_AXI_SI0_WDATA_PARITY</t>
-  </si>
-  <si>
-    <t>ERR_AXICRYPT_AXI_SI0_BUS_PARITY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -209,6 +215,19 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -246,9 +265,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -555,27 +577,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -600,8 +622,8 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
+      <c r="H1" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -615,62 +637,62 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
       <c r="O2">
         <v>36</v>
       </c>
@@ -678,10 +700,10 @@
         <v>36</v>
       </c>
       <c r="Q2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" t="s">
         <v>27</v>
-      </c>
-      <c r="R2" t="s">
-        <v>28</v>
       </c>
       <c r="S2">
         <v>32</v>
@@ -692,31 +714,31 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
       <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O3">
         <v>36</v>
@@ -725,10 +747,10 @@
         <v>36</v>
       </c>
       <c r="Q3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" t="s">
         <v>27</v>
-      </c>
-      <c r="R3" t="s">
-        <v>28</v>
       </c>
       <c r="S3">
         <v>32</v>
@@ -739,37 +761,37 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
         <v>33</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>26</v>
-      </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" t="s">
-        <v>27</v>
       </c>
       <c r="O4">
         <v>256</v>
@@ -778,10 +800,10 @@
         <v>128</v>
       </c>
       <c r="Q4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" t="s">
         <v>27</v>
-      </c>
-      <c r="R4" t="s">
-        <v>28</v>
       </c>
       <c r="S4">
         <v>32</v>
@@ -792,31 +814,31 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
       <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" t="s">
-        <v>36</v>
-      </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O5">
         <v>256</v>
@@ -825,10 +847,10 @@
         <v>128</v>
       </c>
       <c r="Q5" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" t="s">
         <v>27</v>
-      </c>
-      <c r="R5" t="s">
-        <v>28</v>
       </c>
       <c r="S5">
         <v>32</v>
@@ -839,43 +861,43 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6">
+        <v>36</v>
+      </c>
+      <c r="P6">
+        <v>36</v>
+      </c>
+      <c r="Q6" t="s">
         <v>26</v>
       </c>
-      <c r="O6">
-        <v>36</v>
-      </c>
-      <c r="P6">
-        <v>36</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>27</v>
-      </c>
-      <c r="R6" t="s">
-        <v>28</v>
       </c>
       <c r="S6">
         <v>32</v>
@@ -886,43 +908,43 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <v>36</v>
+      </c>
+      <c r="P7">
+        <v>36</v>
+      </c>
+      <c r="Q7" t="s">
         <v>26</v>
       </c>
-      <c r="O7">
-        <v>36</v>
-      </c>
-      <c r="P7">
-        <v>36</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>27</v>
-      </c>
-      <c r="R7" t="s">
-        <v>28</v>
       </c>
       <c r="S7">
         <v>32</v>
@@ -933,37 +955,37 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
         <v>54</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>26</v>
-      </c>
-      <c r="M8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N8" t="s">
-        <v>27</v>
       </c>
       <c r="O8">
         <v>256</v>
@@ -972,10 +994,10 @@
         <v>128</v>
       </c>
       <c r="Q8" t="s">
+        <v>57</v>
+      </c>
+      <c r="R8" t="s">
         <v>27</v>
-      </c>
-      <c r="R8" t="s">
-        <v>28</v>
       </c>
       <c r="S8">
         <v>32</v>
@@ -986,31 +1008,31 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O9">
         <v>256</v>
@@ -1019,10 +1041,10 @@
         <v>128</v>
       </c>
       <c r="Q9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" t="s">
         <v>27</v>
-      </c>
-      <c r="R9" t="s">
-        <v>28</v>
       </c>
       <c r="S9">
         <v>32</v>
@@ -1032,6 +1054,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Before utilizing ENERR and FIERR for receivers
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pnson\Workspace\Parity_Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF34F6C9-3F7B-49C3-9CE7-0E813DA4BB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B86E975-D0B3-4983-B13D-3C6B8B81DD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
   <si>
     <t>VERSION</t>
   </si>
@@ -196,6 +196,10 @@
   </si>
   <si>
     <t>NO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -578,7 +582,7 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -967,7 +971,7 @@
         <v>45</v>
       </c>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Refactor parity assignment logic and remove unnecessary signal assignments
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pnson\Workspace\Parity_Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79FBB9E-BAA5-425F-8942-E422609E1CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD40AC0E-6AD6-4D36-8835-89BF14023B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
   <si>
     <t>VERSION</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>AXICRYPT_AXI_SI0_AWVALID</t>
@@ -582,7 +579,7 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -627,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -642,7 +639,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -689,7 +686,7 @@
         <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
@@ -704,7 +701,7 @@
         <v>36</v>
       </c>
       <c r="Q2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R2" t="s">
         <v>27</v>
@@ -736,7 +733,7 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3" t="s">
         <v>29</v>
@@ -751,7 +748,7 @@
         <v>36</v>
       </c>
       <c r="Q3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R3" t="s">
         <v>27</v>
@@ -783,7 +780,7 @@
         <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
         <v>32</v>
@@ -836,7 +833,7 @@
         <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K5" t="s">
         <v>35</v>
@@ -851,7 +848,7 @@
         <v>128</v>
       </c>
       <c r="Q5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R5" t="s">
         <v>27</v>
@@ -874,19 +871,19 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
         <v>31</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
         <v>25</v>
@@ -921,19 +918,19 @@
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
         <v>31</v>
       </c>
       <c r="J7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" t="s">
         <v>25</v>
@@ -968,25 +965,25 @@
         <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
         <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L8" t="s">
         <v>25</v>
       </c>
       <c r="M8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N8" t="s">
         <v>26</v>
@@ -998,7 +995,7 @@
         <v>128</v>
       </c>
       <c r="Q8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R8" t="s">
         <v>27</v>
@@ -1021,19 +1018,19 @@
         <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
         <v>31</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Fixed top module generation
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pnson\Workspace\Parity_Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B51475-BC72-4AC7-B4DB-E84DC4B55D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39271477-1ECC-4C59-8B37-73F44C70F958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,12 +88,6 @@
     <t>BOS_AXICRYPT</t>
   </si>
   <si>
-    <t>I_CLK</t>
-  </si>
-  <si>
-    <t>I_RESETN</t>
-  </si>
-  <si>
     <t>AXICRYPT_AXI_MI0_ARADDR</t>
   </si>
   <si>
@@ -191,6 +185,12 @@
   </si>
   <si>
     <t>AXICRYPT_AXI_SI0_WDATA_PARITY</t>
+  </si>
+  <si>
+    <t>ACLK</t>
+  </si>
+  <si>
+    <t>RESETN_ACLK</t>
   </si>
 </sst>
 </file>
@@ -571,13 +571,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.625" bestFit="1" customWidth="1"/>
@@ -661,28 +664,28 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>27</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>29</v>
       </c>
       <c r="P2">
         <v>36</v>
@@ -691,7 +694,7 @@
         <v>36</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S2">
         <v>32</v>
@@ -705,28 +708,28 @@
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" t="s">
-        <v>33</v>
-      </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P3">
         <v>36</v>
@@ -735,7 +738,7 @@
         <v>36</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S3">
         <v>32</v>
@@ -749,34 +752,34 @@
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>35</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
         <v>36</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>37</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" t="s">
-        <v>39</v>
       </c>
       <c r="P4">
         <v>256</v>
@@ -785,7 +788,7 @@
         <v>128</v>
       </c>
       <c r="R4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S4">
         <v>32</v>
@@ -799,28 +802,28 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
         <v>40</v>
       </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" t="s">
-        <v>42</v>
-      </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P5">
         <v>256</v>
@@ -829,7 +832,7 @@
         <v>128</v>
       </c>
       <c r="R5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S5">
         <v>32</v>
@@ -843,28 +846,28 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
         <v>43</v>
       </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" t="s">
-        <v>45</v>
-      </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P6">
         <v>36</v>
@@ -873,7 +876,7 @@
         <v>36</v>
       </c>
       <c r="R6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S6">
         <v>32</v>
@@ -887,28 +890,28 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
         <v>46</v>
       </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" t="s">
-        <v>47</v>
-      </c>
-      <c r="L7" t="s">
-        <v>48</v>
-      </c>
       <c r="M7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P7">
         <v>36</v>
@@ -917,7 +920,7 @@
         <v>36</v>
       </c>
       <c r="R7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S7">
         <v>32</v>
@@ -931,34 +934,34 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
         <v>49</v>
       </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" t="s">
         <v>50</v>
       </c>
-      <c r="L8" t="s">
-        <v>51</v>
-      </c>
-      <c r="M8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" t="s">
-        <v>52</v>
-      </c>
       <c r="O8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="P8">
         <v>256</v>
@@ -967,7 +970,7 @@
         <v>128</v>
       </c>
       <c r="R8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S8">
         <v>32</v>
@@ -981,28 +984,28 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" t="s">
         <v>53</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
         <v>54</v>
       </c>
-      <c r="J9" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" t="s">
-        <v>56</v>
-      </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P9">
         <v>256</v>
@@ -1011,7 +1014,7 @@
         <v>128</v>
       </c>
       <c r="R9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S9">
         <v>32</v>

</xml_diff>

<commit_message>
Correctly top module overwirte method
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pnson\Workspace\Parity_Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39271477-1ECC-4C59-8B37-73F44C70F958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F7C9BD-247F-4AF8-BDB6-40AB28CF113C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,9 +178,6 @@
     <t>AXICRYPT_AXI_SI0_WDATA</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>AXICRYPT_AXI_SI0_WVALID</t>
   </si>
   <si>
@@ -191,6 +188,10 @@
   </si>
   <si>
     <t>RESETN_ACLK</t>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -572,7 +573,7 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -664,10 +665,10 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
         <v>55</v>
-      </c>
-      <c r="G2" t="s">
-        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>22</v>
@@ -708,10 +709,10 @@
         <v>21</v>
       </c>
       <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
         <v>55</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -752,10 +753,10 @@
         <v>21</v>
       </c>
       <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
         <v>55</v>
-      </c>
-      <c r="G4" t="s">
-        <v>56</v>
       </c>
       <c r="H4" t="s">
         <v>32</v>
@@ -802,10 +803,10 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
         <v>55</v>
-      </c>
-      <c r="G5" t="s">
-        <v>56</v>
       </c>
       <c r="H5" t="s">
         <v>38</v>
@@ -846,10 +847,10 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
         <v>55</v>
-      </c>
-      <c r="G6" t="s">
-        <v>56</v>
       </c>
       <c r="H6" t="s">
         <v>41</v>
@@ -890,10 +891,10 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
         <v>55</v>
-      </c>
-      <c r="G7" t="s">
-        <v>56</v>
       </c>
       <c r="H7" t="s">
         <v>44</v>
@@ -934,10 +935,10 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
         <v>55</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
       </c>
       <c r="H8" t="s">
         <v>47</v>
@@ -984,25 +985,25 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
         <v>55</v>
-      </c>
-      <c r="G9" t="s">
-        <v>56</v>
       </c>
       <c r="H9" t="s">
         <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="J9" t="s">
         <v>33</v>
       </c>
       <c r="K9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" t="s">
         <v>53</v>
-      </c>
-      <c r="L9" t="s">
-        <v>54</v>
       </c>
       <c r="M9" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Fix MD5 calculation per GROUP and correct writing position to MD5 column in INFO file
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -452,10 +452,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V9"/>
+  <dimension ref="A2:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -476,186 +476,118 @@
     <col width="9.5" bestFit="1" customWidth="1" min="18" max="18"/>
     <col width="25.25" bestFit="1" customWidth="1" min="19" max="19"/>
     <col width="19" bestFit="1" customWidth="1" min="20" max="20"/>
+    <col width="56.125" bestFit="1" customWidth="1" min="21" max="21"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>VERSION</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>HSR ID</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>SM ID</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>IP NAME</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>CLOCK</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G2" s="1" t="inlineStr">
         <is>
           <t>RESET</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>SIGNAL PORT NAME</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>GROUP</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J2" s="1" t="inlineStr">
         <is>
           <t>DRIVE/RECEIVE</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>SIGNAL VALID NAME</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L2" s="1" t="inlineStr">
         <is>
           <t>PARITY PORT NAME</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>IP FILE LIST</t>
         </is>
       </c>
-      <c r="N1" s="2" t="inlineStr">
+      <c r="N2" s="2" t="inlineStr">
         <is>
           <t>ERROR PORT</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>ERROR DOUBLE</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>BIT WIDTH</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q2" s="1" t="inlineStr">
         <is>
           <t>PARITY SOURCE BIT WIDTH</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R2" s="1" t="inlineStr">
         <is>
           <t>EVEN ODD</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S2" s="1" t="inlineStr">
         <is>
           <t>COMPARATOR INPUT WIDTH</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T2" s="1" t="inlineStr">
         <is>
           <t>COMPARATOR DEPTH</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="U2" s="1" t="inlineStr">
         <is>
           <t>MD5 &amp; Script Version</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V2" s="1" t="inlineStr">
         <is>
           <t>NOTE</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>BOS_AXICRYPT</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>ACLK</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>RESETN_ACLK</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>AXICRYPT_AXI_MI0_ARADDR</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>DRIVE</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>AXICRYPT_AXI_MI0_ARVALID</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>AXICRYPT_AXI_MI0_ARADDR_PARITY</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>$AXICRYPT_HOME/RTL/filelist.f</t>
-        </is>
-      </c>
-      <c r="P2" t="n">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>36</v>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>EVEN</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>32</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -677,7 +609,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_AWADDR</t>
+          <t>AXICRYPT_AXI_MI0_ARADDR</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -692,12 +624,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_AWVALID</t>
+          <t>AXICRYPT_AXI_MI0_ARVALID</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_AWADDR_PARITY</t>
+          <t>AXICRYPT_AXI_MI0_ARADDR_PARITY</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -724,7 +656,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>MD5: dd4192493b15e873de59e66662701d9c | Script: v3.0.0</t>
+          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -746,7 +678,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_RDATA</t>
+          <t>AXICRYPT_AXI_MI0_AWADDR</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -756,17 +688,17 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>RECEIVE</t>
+          <t>DRIVE</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_RVALID</t>
+          <t>AXICRYPT_AXI_MI0_AWVALID</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_RDATA_PARITY</t>
+          <t>AXICRYPT_AXI_MI0_AWADDR_PARITY</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -774,21 +706,11 @@
           <t>$AXICRYPT_HOME/RTL/filelist.f</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>ERR_AXICRYPT_AXI_MI0_BUS_PARITY</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
       <c r="P4" t="n">
-        <v>256</v>
+        <v>36</v>
       </c>
       <c r="Q4" t="n">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
@@ -803,7 +725,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>MD5: c46f761ea3b38048c33031cbec0299c0 | Script: v3.0.0</t>
+          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -825,7 +747,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_WDATA</t>
+          <t>AXICRYPT_AXI_MI0_RDATA</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -835,22 +757,32 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>DRIVE</t>
+          <t>RECEIVE</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_WVALID</t>
+          <t>AXICRYPT_AXI_MI0_RVALID</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_MI0_WDATA_PARITY</t>
+          <t>AXICRYPT_AXI_MI0_RDATA_PARITY</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
           <t>$AXICRYPT_HOME/RTL/filelist.f</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>ERR_AXICRYPT_AXI_MI0_BUS_PARITY</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="P5" t="n">
@@ -872,7 +804,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>MD5: 94ad3caffd6a4f386d7f849585f8ad13 | Script: v3.0.0</t>
+          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -894,7 +826,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_ARADDR</t>
+          <t>AXICRYPT_AXI_MI0_WDATA</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -904,17 +836,17 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>RECEIVE</t>
+          <t>DRIVE</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_ARVALID</t>
+          <t>AXICRYPT_AXI_MI0_WVALID</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_ARADDR_PARITY</t>
+          <t>AXICRYPT_AXI_MI0_WDATA_PARITY</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -923,10 +855,10 @@
         </is>
       </c>
       <c r="P6" t="n">
-        <v>36</v>
+        <v>256</v>
       </c>
       <c r="Q6" t="n">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="R6" t="inlineStr">
         <is>
@@ -941,7 +873,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>MD5: 6fef528639263f9043a09083e52b7230 | Script: v3.0.0</t>
+          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -963,7 +895,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_AWADDR</t>
+          <t>AXICRYPT_AXI_SI0_ARADDR</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -978,12 +910,12 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_AWVALID</t>
+          <t>AXICRYPT_AXI_SI0_ARVALID</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_AWADDR_PARITY</t>
+          <t>AXICRYPT_AXI_SI0_ARADDR_PARITY</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1010,7 +942,7 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>MD5: a340a3abb1c6a10321d2be53deace048 | Script: v3.0.0</t>
+          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -1032,7 +964,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_RDATA</t>
+          <t>AXICRYPT_AXI_SI0_AWADDR</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1042,17 +974,17 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>DRIVE</t>
+          <t>RECEIVE</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_RVALID</t>
+          <t>AXICRYPT_AXI_SI0_AWVALID</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_RDATA_PARITY</t>
+          <t>AXICRYPT_AXI_SI0_AWADDR_PARITY</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1060,21 +992,11 @@
           <t>$AXICRYPT_HOME/RTL/filelist.f</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>ERR_AXICRYPT_AXI_SI0_BUS_PARITY</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
       <c r="P8" t="n">
-        <v>256</v>
+        <v>36</v>
       </c>
       <c r="Q8" t="n">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
@@ -1089,7 +1011,7 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>MD5: b50a9102a76d0b584078823dab985d2b | Script: v3.0.0</t>
+          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1033,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_WDATA</t>
+          <t>AXICRYPT_AXI_SI0_RDATA</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1121,22 +1043,32 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>RECEIVE</t>
+          <t>DRIVE</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_WVALID</t>
+          <t>AXICRYPT_AXI_SI0_RVALID</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>AXICRYPT_AXI_SI0_WDATA_PARITY</t>
+          <t>AXICRYPT_AXI_SI0_RDATA_PARITY</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
           <t>$AXICRYPT_HOME/RTL/filelist.f</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>ERR_AXICRYPT_AXI_SI0_BUS_PARITY</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>YES</t>
         </is>
       </c>
       <c r="P9" t="n">
@@ -1158,7 +1090,76 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>MD5: 8e7a8c84a3dc3ce0bc1e231debd245e1 | Script: v3.0.0</t>
+          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>BOS_AXICRYPT</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ACLK</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>RESETN_ACLK</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>AXICRYPT_AXI_SI0_WDATA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>RECEIVE</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>AXICRYPT_AXI_SI0_WVALID</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>AXICRYPT_AXI_SI0_WDATA_PARITY</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>$AXICRYPT_HOME/RTL/filelist.f</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>256</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>128</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>EVEN</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>32</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP: Improve gen_top logic to preserve original module structure and add parity ports/instance
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SAFETY.PARITY" sheetId="1" state="visible" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="A2:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -638,10 +638,10 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q3" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -656,7 +656,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+          <t>MD5: 0361ade3b14b1220359a6cc5e306a61e | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -707,10 +707,10 @@
         </is>
       </c>
       <c r="P4" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q4" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
@@ -725,7 +725,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+          <t>MD5: 0361ade3b14b1220359a6cc5e306a61e | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
         <v>256</v>
       </c>
       <c r="Q5" t="n">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
@@ -804,7 +804,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+          <t>MD5: 0361ade3b14b1220359a6cc5e306a61e | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -858,7 +858,7 @@
         <v>256</v>
       </c>
       <c r="Q6" t="n">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="R6" t="inlineStr">
         <is>
@@ -873,7 +873,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+          <t>MD5: 0361ade3b14b1220359a6cc5e306a61e | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -924,10 +924,10 @@
         </is>
       </c>
       <c r="P7" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q7" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="R7" t="inlineStr">
         <is>
@@ -942,7 +942,7 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+          <t>MD5: 0361ade3b14b1220359a6cc5e306a61e | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -993,10 +993,10 @@
         </is>
       </c>
       <c r="P8" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q8" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+          <t>MD5: 0361ade3b14b1220359a6cc5e306a61e | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
         <v>256</v>
       </c>
       <c r="Q9" t="n">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="R9" t="inlineStr">
         <is>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+          <t>MD5: 0361ade3b14b1220359a6cc5e306a61e | Script: v3.0.0</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1144,7 @@
         <v>256</v>
       </c>
       <c r="Q10" t="n">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="R10" t="inlineStr">
         <is>
@@ -1159,11 +1159,12 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>MD5: d4f6fa9523038fdb5e8b258d4c9d18c4 | Script: v3.0.0</t>
+          <t>MD5: 0361ade3b14b1220359a6cc5e306a61e | Script: v3.0.0</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: Remove old parity control ports from module declaration
- Enhanced clean_parity_from_module to remove old MI0/SI0 specific error ports
- Removed FIERR_AXICRYPT_AXI_MI0/SI0_* ports (replaced by new consolidated format)
- Removed ENERR_AXICRYPT_AXI_MI0/SI0_* ports (replaced by consolidated format)
- Removed old ERR_AXICRYPT_AXI_MI0_BUS_PARITY_B (replaced by ERR_AXICRYPT_AXI_BUS_PARITY_B)
- Result: NEW files now have clean parity port declarations matching the new generator design
- Kept: Core logic error ports (DCLS), new consolidated error format ports
</commit_message>
<xml_diff>
--- a/[INFO]_BOS_AXICRYPT.safety.xlsx
+++ b/[INFO]_BOS_AXICRYPT.safety.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-210" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SAFETY.PARITY" sheetId="1" state="visible" r:id="rId1"/>
@@ -454,8 +454,8 @@
   </sheetPr>
   <dimension ref="A2:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -777,7 +777,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>ERR_AXICRYPT_AXI_MI0_BUS_PARITY</t>
+          <t>ERR_AXICRYPT_AXI_BUS_PARITY</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">

</xml_diff>